<commit_message>
Full contact angle dataset
Reanalyze contact angle data now that all images have been processed. Plot contact angle differences within each population pair.
</commit_message>
<xml_diff>
--- a/Data/Contact Angle Measurements.xlsx
+++ b/Data/Contact Angle Measurements.xlsx
@@ -1435,6 +1435,12 @@
       <c r="D11" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="E11" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>61.13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
@@ -1449,6 +1455,12 @@
       <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E12" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>63.67</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
@@ -5223,6 +5235,12 @@
       <c r="D201" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="E201" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F201" s="4">
+        <v>58.62</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="s">
@@ -5237,6 +5255,12 @@
       <c r="D202" s="1" t="s">
         <v>218</v>
       </c>
+      <c r="E202" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F202" s="4">
+        <v>61.56</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="s">
@@ -5251,6 +5275,12 @@
       <c r="D203" s="1" t="s">
         <v>219</v>
       </c>
+      <c r="E203" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F203" s="4">
+        <v>61.47</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="s">
@@ -5265,6 +5295,12 @@
       <c r="D204" s="1" t="s">
         <v>220</v>
       </c>
+      <c r="E204" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F204" s="4">
+        <v>57.11</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="s">
@@ -5279,6 +5315,12 @@
       <c r="D205" s="1" t="s">
         <v>221</v>
       </c>
+      <c r="E205" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F205" s="4">
+        <v>59.25</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="s">
@@ -5293,6 +5335,12 @@
       <c r="D206" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="E206" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F206" s="4">
+        <v>57.59</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="s">
@@ -5307,6 +5355,12 @@
       <c r="D207" s="1" t="s">
         <v>223</v>
       </c>
+      <c r="E207" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F207" s="4">
+        <v>53.59</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="s">
@@ -5321,6 +5375,12 @@
       <c r="D208" s="1" t="s">
         <v>224</v>
       </c>
+      <c r="E208" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F208" s="4">
+        <v>64.75</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="s">
@@ -5335,6 +5395,12 @@
       <c r="D209" s="1" t="s">
         <v>225</v>
       </c>
+      <c r="E209" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F209" s="4">
+        <v>53.39</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="s">
@@ -5349,6 +5415,12 @@
       <c r="D210" s="1" t="s">
         <v>226</v>
       </c>
+      <c r="E210" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F210" s="4">
+        <v>64.19</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="s">
@@ -5363,6 +5435,12 @@
       <c r="D211" s="1" t="s">
         <v>227</v>
       </c>
+      <c r="E211" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F211" s="4">
+        <v>63.97</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="s">
@@ -5377,6 +5455,12 @@
       <c r="D212" s="1" t="s">
         <v>228</v>
       </c>
+      <c r="E212" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F212" s="4">
+        <v>60.65</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="s">
@@ -5391,6 +5475,12 @@
       <c r="D213" s="1" t="s">
         <v>229</v>
       </c>
+      <c r="E213" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F213" s="4">
+        <v>58.68</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="s">
@@ -5405,6 +5495,12 @@
       <c r="D214" s="1" t="s">
         <v>230</v>
       </c>
+      <c r="E214" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F214" s="4">
+        <v>58.61</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="s">
@@ -5419,6 +5515,12 @@
       <c r="D215" s="1" t="s">
         <v>231</v>
       </c>
+      <c r="E215" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F215" s="4">
+        <v>53.31</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="s">
@@ -5433,6 +5535,12 @@
       <c r="D216" s="1" t="s">
         <v>232</v>
       </c>
+      <c r="E216" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F216" s="4">
+        <v>65.28</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="s">
@@ -5447,6 +5555,12 @@
       <c r="D217" s="1" t="s">
         <v>233</v>
       </c>
+      <c r="E217" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F217" s="4">
+        <v>60.51</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="s">
@@ -5461,6 +5575,12 @@
       <c r="D218" s="1" t="s">
         <v>234</v>
       </c>
+      <c r="E218" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F218" s="4">
+        <v>62.15</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="s">
@@ -5475,6 +5595,12 @@
       <c r="D219" s="1" t="s">
         <v>235</v>
       </c>
+      <c r="E219" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F219" s="4">
+        <v>57.66</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
@@ -5489,6 +5615,12 @@
       <c r="D220" s="1" t="s">
         <v>236</v>
       </c>
+      <c r="E220" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F220" s="4">
+        <v>70.9</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
@@ -5503,6 +5635,12 @@
       <c r="D221" s="1" t="s">
         <v>237</v>
       </c>
+      <c r="E221" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F221" s="4">
+        <v>62.73</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
@@ -5517,6 +5655,12 @@
       <c r="D222" s="1" t="s">
         <v>238</v>
       </c>
+      <c r="E222" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F222" s="4">
+        <v>62.39</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
@@ -5531,6 +5675,12 @@
       <c r="D223" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="E223" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F223" s="4">
+        <v>69.67</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
@@ -5545,6 +5695,12 @@
       <c r="D224" s="1" t="s">
         <v>240</v>
       </c>
+      <c r="E224" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F224" s="4">
+        <v>59.34</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
@@ -5559,6 +5715,12 @@
       <c r="D225" s="1" t="s">
         <v>241</v>
       </c>
+      <c r="E225" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F225" s="4">
+        <v>68.0</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
@@ -5573,6 +5735,12 @@
       <c r="D226" s="1" t="s">
         <v>242</v>
       </c>
+      <c r="E226" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F226" s="4">
+        <v>68.06</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
@@ -5587,6 +5755,12 @@
       <c r="D227" s="1" t="s">
         <v>243</v>
       </c>
+      <c r="E227" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F227" s="4">
+        <v>76.21</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
@@ -5601,6 +5775,12 @@
       <c r="D228" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="E228" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F228" s="4">
+        <v>58.58</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
@@ -5615,6 +5795,12 @@
       <c r="D229" s="1" t="s">
         <v>245</v>
       </c>
+      <c r="E229" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F229" s="4">
+        <v>54.56</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
@@ -5629,6 +5815,12 @@
       <c r="D230" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="E230" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F230" s="4">
+        <v>31.34</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
@@ -5643,6 +5835,12 @@
       <c r="D231" s="1" t="s">
         <v>247</v>
       </c>
+      <c r="E231" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F231" s="4">
+        <v>55.82</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
@@ -5657,6 +5855,12 @@
       <c r="D232" s="1" t="s">
         <v>248</v>
       </c>
+      <c r="E232" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F232" s="4">
+        <v>41.02</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
@@ -5671,6 +5875,12 @@
       <c r="D233" s="1" t="s">
         <v>249</v>
       </c>
+      <c r="E233" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F233" s="4">
+        <v>59.82</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
@@ -5685,6 +5895,12 @@
       <c r="D234" s="1" t="s">
         <v>250</v>
       </c>
+      <c r="E234" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F234" s="4">
+        <v>54.89</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
@@ -5699,6 +5915,12 @@
       <c r="D235" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="E235" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F235" s="4">
+        <v>57.23</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
@@ -5713,6 +5935,12 @@
       <c r="D236" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="E236" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F236" s="4">
+        <v>68.71</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
@@ -5727,6 +5955,12 @@
       <c r="D237" s="1" t="s">
         <v>253</v>
       </c>
+      <c r="E237" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F237" s="4">
+        <v>58.3</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
@@ -5741,6 +5975,12 @@
       <c r="D238" s="1" t="s">
         <v>254</v>
       </c>
+      <c r="E238" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F238" s="4">
+        <v>67.82</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
@@ -5755,6 +5995,12 @@
       <c r="D239" s="1" t="s">
         <v>255</v>
       </c>
+      <c r="E239" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F239" s="4">
+        <v>69.51</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
@@ -5769,6 +6015,12 @@
       <c r="D240" s="1" t="s">
         <v>256</v>
       </c>
+      <c r="E240" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F240" s="4">
+        <v>58.68</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
@@ -5783,6 +6035,12 @@
       <c r="D241" s="1" t="s">
         <v>257</v>
       </c>
+      <c r="E241" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F241" s="4">
+        <v>55.07</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
@@ -5797,6 +6055,12 @@
       <c r="D242" s="1" t="s">
         <v>258</v>
       </c>
+      <c r="E242" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F242" s="4">
+        <v>59.96</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="s">
@@ -5811,6 +6075,12 @@
       <c r="D243" s="1" t="s">
         <v>259</v>
       </c>
+      <c r="E243" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F243" s="4">
+        <v>58.23</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
@@ -5825,6 +6095,12 @@
       <c r="D244" s="1" t="s">
         <v>260</v>
       </c>
+      <c r="E244" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F244" s="4">
+        <v>35.97</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="s">
@@ -5839,6 +6115,12 @@
       <c r="D245" s="1" t="s">
         <v>261</v>
       </c>
+      <c r="E245" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F245" s="4">
+        <v>50.41</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="s">
@@ -5853,6 +6135,12 @@
       <c r="D246" s="1" t="s">
         <v>262</v>
       </c>
+      <c r="E246" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F246" s="4">
+        <v>58.65</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="s">
@@ -5867,6 +6155,12 @@
       <c r="D247" s="1" t="s">
         <v>263</v>
       </c>
+      <c r="E247" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F247" s="4">
+        <v>56.57</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="s">
@@ -5881,6 +6175,12 @@
       <c r="D248" s="1" t="s">
         <v>264</v>
       </c>
+      <c r="E248" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F248" s="4">
+        <v>33.09</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="s">
@@ -5895,6 +6195,12 @@
       <c r="D249" s="1" t="s">
         <v>265</v>
       </c>
+      <c r="E249" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F249" s="4">
+        <v>33.09</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="s">
@@ -5909,6 +6215,12 @@
       <c r="D250" s="1" t="s">
         <v>266</v>
       </c>
+      <c r="E250" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F250" s="4">
+        <v>71.45</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
@@ -5923,6 +6235,12 @@
       <c r="D251" s="1" t="s">
         <v>267</v>
       </c>
+      <c r="E251" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F251" s="4">
+        <v>16.57</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="s">
@@ -5937,6 +6255,12 @@
       <c r="D252" s="1" t="s">
         <v>268</v>
       </c>
+      <c r="E252" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F252" s="4">
+        <v>75.96</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="s">
@@ -5951,6 +6275,12 @@
       <c r="D253" s="1" t="s">
         <v>269</v>
       </c>
+      <c r="E253" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F253" s="4">
+        <v>54.17</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="s">
@@ -5965,6 +6295,12 @@
       <c r="D254" s="1" t="s">
         <v>270</v>
       </c>
+      <c r="E254" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F254" s="4">
+        <v>59.36</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="s">
@@ -5979,6 +6315,12 @@
       <c r="D255" s="1" t="s">
         <v>271</v>
       </c>
+      <c r="E255" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F255" s="4">
+        <v>69.54</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="s">
@@ -5993,6 +6335,12 @@
       <c r="D256" s="1" t="s">
         <v>272</v>
       </c>
+      <c r="E256" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F256" s="4">
+        <v>45.45</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="s">
@@ -6007,6 +6355,12 @@
       <c r="D257" s="1" t="s">
         <v>273</v>
       </c>
+      <c r="E257" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F257" s="4">
+        <v>61.16</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="s">
@@ -6021,6 +6375,12 @@
       <c r="D258" s="1" t="s">
         <v>274</v>
       </c>
+      <c r="E258" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F258" s="4">
+        <v>67.81</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="s">
@@ -6035,6 +6395,12 @@
       <c r="D259" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="E259" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F259" s="4">
+        <v>68.97</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="s">
@@ -6049,6 +6415,12 @@
       <c r="D260" s="1" t="s">
         <v>276</v>
       </c>
+      <c r="E260" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F260" s="4">
+        <v>59.9</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="s">
@@ -6063,6 +6435,12 @@
       <c r="D261" s="1" t="s">
         <v>277</v>
       </c>
+      <c r="E261" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F261" s="4">
+        <v>69.06</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="s">
@@ -6077,6 +6455,12 @@
       <c r="D262" s="1" t="s">
         <v>278</v>
       </c>
+      <c r="E262" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F262" s="4">
+        <v>68.08</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="s">
@@ -6091,6 +6475,12 @@
       <c r="D263" s="1" t="s">
         <v>279</v>
       </c>
+      <c r="E263" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F263" s="4">
+        <v>42.34</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="s">
@@ -6105,6 +6495,12 @@
       <c r="D264" s="1" t="s">
         <v>280</v>
       </c>
+      <c r="E264" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F264" s="4">
+        <v>58.25</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
@@ -6119,6 +6515,12 @@
       <c r="D265" s="1" t="s">
         <v>281</v>
       </c>
+      <c r="E265" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F265" s="4">
+        <v>56.41</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
@@ -6133,6 +6535,12 @@
       <c r="D266" s="1" t="s">
         <v>282</v>
       </c>
+      <c r="E266" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F266" s="4">
+        <v>77.94</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
@@ -6147,6 +6555,12 @@
       <c r="D267" s="1" t="s">
         <v>283</v>
       </c>
+      <c r="E267" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F267" s="4">
+        <v>74.05</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
@@ -6161,6 +6575,12 @@
       <c r="D268" s="1" t="s">
         <v>284</v>
       </c>
+      <c r="E268" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F268" s="4">
+        <v>66.08</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
@@ -6175,6 +6595,12 @@
       <c r="D269" s="1" t="s">
         <v>285</v>
       </c>
+      <c r="E269" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F269" s="4">
+        <v>43.54</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
@@ -6189,6 +6615,12 @@
       <c r="D270" s="1" t="s">
         <v>286</v>
       </c>
+      <c r="E270" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F270" s="4">
+        <v>50.44</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
@@ -6203,6 +6635,12 @@
       <c r="D271" s="1" t="s">
         <v>287</v>
       </c>
+      <c r="E271" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F271" s="4">
+        <v>51.75</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
@@ -6217,6 +6655,12 @@
       <c r="D272" s="1" t="s">
         <v>288</v>
       </c>
+      <c r="E272" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F272" s="4">
+        <v>70.96</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
@@ -6231,6 +6675,12 @@
       <c r="D273" s="1" t="s">
         <v>289</v>
       </c>
+      <c r="E273" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F273" s="4">
+        <v>66.29</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="s">
@@ -6245,6 +6695,12 @@
       <c r="D274" s="1" t="s">
         <v>290</v>
       </c>
+      <c r="E274" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F274" s="4">
+        <v>60.42</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="s">
@@ -6259,6 +6715,12 @@
       <c r="D275" s="1" t="s">
         <v>291</v>
       </c>
+      <c r="E275" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F275" s="4">
+        <v>42.34</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
@@ -6287,6 +6749,12 @@
       <c r="D277" s="1" t="s">
         <v>293</v>
       </c>
+      <c r="E277" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F277" s="4">
+        <v>61.95</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
@@ -6301,6 +6769,12 @@
       <c r="D278" s="1" t="s">
         <v>294</v>
       </c>
+      <c r="E278" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F278" s="4">
+        <v>62.51</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
@@ -6315,6 +6789,12 @@
       <c r="D279" s="1" t="s">
         <v>295</v>
       </c>
+      <c r="E279" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F279" s="4">
+        <v>52.66</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
@@ -6329,6 +6809,12 @@
       <c r="D280" s="1" t="s">
         <v>296</v>
       </c>
+      <c r="E280" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F280" s="4">
+        <v>55.31</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
@@ -6343,6 +6829,12 @@
       <c r="D281" s="1" t="s">
         <v>297</v>
       </c>
+      <c r="E281" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F281" s="4">
+        <v>41.51</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
@@ -6357,6 +6849,12 @@
       <c r="D282" s="1" t="s">
         <v>298</v>
       </c>
+      <c r="E282" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F282" s="4">
+        <v>69.9</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
@@ -6371,6 +6869,12 @@
       <c r="D283" s="1" t="s">
         <v>299</v>
       </c>
+      <c r="E283" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F283" s="4">
+        <v>54.32</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
@@ -6385,6 +6889,12 @@
       <c r="D284" s="1" t="s">
         <v>300</v>
       </c>
+      <c r="E284" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F284" s="4">
+        <v>80.92</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
@@ -6399,6 +6909,12 @@
       <c r="D285" s="1" t="s">
         <v>301</v>
       </c>
+      <c r="E285" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F285" s="4">
+        <v>70.53</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
@@ -6413,6 +6929,12 @@
       <c r="D286" s="1" t="s">
         <v>302</v>
       </c>
+      <c r="E286" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F286" s="4">
+        <v>56.85</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
@@ -6427,6 +6949,12 @@
       <c r="D287" s="1" t="s">
         <v>303</v>
       </c>
+      <c r="E287" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F287" s="4">
+        <v>51.48</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
@@ -6441,6 +6969,12 @@
       <c r="D288" s="1" t="s">
         <v>304</v>
       </c>
+      <c r="E288" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F288" s="4">
+        <v>75.05</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
@@ -6455,6 +6989,12 @@
       <c r="D289" s="1" t="s">
         <v>305</v>
       </c>
+      <c r="E289" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F289" s="4">
+        <v>60.82</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
@@ -6469,6 +7009,12 @@
       <c r="D290" s="1" t="s">
         <v>306</v>
       </c>
+      <c r="E290" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F290" s="4">
+        <v>75.87</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
@@ -6483,6 +7029,12 @@
       <c r="D291" s="1" t="s">
         <v>307</v>
       </c>
+      <c r="E291" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F291" s="4">
+        <v>65.83</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
@@ -6497,6 +7049,12 @@
       <c r="D292" s="1" t="s">
         <v>308</v>
       </c>
+      <c r="E292" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F292" s="4">
+        <v>74.39</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
@@ -6511,6 +7069,12 @@
       <c r="D293" s="1" t="s">
         <v>309</v>
       </c>
+      <c r="E293" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F293" s="4">
+        <v>62.47</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
@@ -6525,6 +7089,12 @@
       <c r="D294" s="1" t="s">
         <v>310</v>
       </c>
+      <c r="E294" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F294" s="4">
+        <v>66.28</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
@@ -6539,6 +7109,12 @@
       <c r="D295" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="E295" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F295" s="4">
+        <v>67.42</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
@@ -6552,6 +7128,12 @@
       </c>
       <c r="D296" s="1" t="s">
         <v>312</v>
+      </c>
+      <c r="E296" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F296" s="4">
+        <v>73.12</v>
       </c>
     </row>
     <row r="297">

</xml_diff>